<commit_message>
Updating split Excel sheets table
</commit_message>
<xml_diff>
--- a/Split Excel Sheet Into Multiple Sheets/InputData.xlsx
+++ b/Split Excel Sheet Into Multiple Sheets/InputData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Hall\Documents\UiPath\UpdatedTemplates\Split Excel Sheet into Multiple Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Hall\Source\repos\StudioXTemplates\Split Excel Sheet Into Multiple Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3671EA-C801-49D1-8F11-0EFAF5C104F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765CCA66-3180-443B-BC35-41864C8F4D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1284" yWindow="-108" windowWidth="29544" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3015" yWindow="3315" windowWidth="20550" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,14 +483,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +504,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -518,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -532,7 +532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -546,7 +546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -560,7 +560,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -574,7 +574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -588,7 +588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -602,7 +602,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -616,7 +616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -630,7 +630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -644,7 +644,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -658,7 +658,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>

</xml_diff>